<commit_message>
Adding a new Agent test case
</commit_message>
<xml_diff>
--- a/data/TestData.xlsx
+++ b/data/TestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27022"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="51120" windowHeight="28360" tabRatio="500"/>
+    <workbookView xWindow="1500" yWindow="0" windowWidth="28560" windowHeight="28320" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="TestCases" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="48">
   <si>
     <t>Runmode</t>
   </si>
@@ -31,9 +31,6 @@
     <t>Y</t>
   </si>
   <si>
-    <t>Chrome</t>
-  </si>
-  <si>
     <t>TCID</t>
   </si>
   <si>
@@ -46,9 +43,6 @@
     <t>DataKey</t>
   </si>
   <si>
-    <t>LoginTest</t>
-  </si>
-  <si>
     <t>openBrowser</t>
   </si>
   <si>
@@ -58,39 +52,18 @@
     <t>verifyTitle</t>
   </si>
   <si>
-    <t>isElementPresent</t>
-  </si>
-  <si>
     <t>click</t>
   </si>
   <si>
     <t>input</t>
   </si>
   <si>
-    <t xml:space="preserve">input </t>
-  </si>
-  <si>
-    <t>exitFrame</t>
-  </si>
-  <si>
     <t>url</t>
   </si>
   <si>
     <t>homePageTitle</t>
   </si>
   <si>
-    <t>signLink_xpath</t>
-  </si>
-  <si>
-    <t>loginUsername_id</t>
-  </si>
-  <si>
-    <t>loginPassword_id</t>
-  </si>
-  <si>
-    <t>submitButton_xpath</t>
-  </si>
-  <si>
     <t>Username</t>
   </si>
   <si>
@@ -106,9 +79,6 @@
     <t>Pass</t>
   </si>
   <si>
-    <t>IE</t>
-  </si>
-  <si>
     <t>N</t>
   </si>
   <si>
@@ -124,56 +94,83 @@
     <t>CreateLeadTest</t>
   </si>
   <si>
-    <t>crmLink_xpath</t>
-  </si>
-  <si>
-    <t>createLew_xpath</t>
-  </si>
-  <si>
-    <t>newLead_xpath</t>
-  </si>
-  <si>
-    <t>firstname_xpath</t>
-  </si>
-  <si>
-    <t>company_xpath</t>
-  </si>
-  <si>
-    <t>FirstName</t>
-  </si>
-  <si>
-    <t>Company</t>
-  </si>
-  <si>
-    <t>LastName</t>
-  </si>
-  <si>
-    <t>lastname_xpath</t>
-  </si>
-  <si>
-    <t>userOne</t>
-  </si>
-  <si>
-    <t>userTwo</t>
-  </si>
-  <si>
-    <t>passwordOne</t>
-  </si>
-  <si>
-    <t>passwordTwo</t>
-  </si>
-  <si>
     <t>cheatButton_id</t>
   </si>
   <si>
     <t>AgentAppGiAk</t>
+  </si>
+  <si>
+    <t>AgentId_id</t>
+  </si>
+  <si>
+    <t>AgentName_id</t>
+  </si>
+  <si>
+    <t>AgentFullName</t>
+  </si>
+  <si>
+    <t>Tom Corless</t>
+  </si>
+  <si>
+    <t>testauto</t>
+  </si>
+  <si>
+    <t>ZipCode_id</t>
+  </si>
+  <si>
+    <t>DOB_id</t>
+  </si>
+  <si>
+    <t>MPBED_id</t>
+  </si>
+  <si>
+    <t>stateZip</t>
+  </si>
+  <si>
+    <t>Dob</t>
+  </si>
+  <si>
+    <t>mpbed</t>
+  </si>
+  <si>
+    <t>1/1/1945</t>
+  </si>
+  <si>
+    <t>A_id</t>
+  </si>
+  <si>
+    <t>ReqEffectiveDate_id</t>
+  </si>
+  <si>
+    <t>select</t>
+  </si>
+  <si>
+    <t>dpsd</t>
+  </si>
+  <si>
+    <t>waitForSpecificSeconds</t>
+  </si>
+  <si>
+    <t>99501</t>
+  </si>
+  <si>
+    <t>nextStep_cssSelector</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>02/01/2017</t>
+  </si>
+  <si>
+    <t>1/1/2015</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -220,6 +217,11 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Menlo"/>
     </font>
   </fonts>
   <fills count="4">
@@ -277,7 +279,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="9">
+  <cellStyleXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -287,13 +289,43 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -306,16 +338,57 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="9">
+  <cellStyles count="41">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -645,43 +718,43 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E22"/>
+  <dimension ref="A1:E24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="13.83203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="18.6640625" customWidth="1"/>
-    <col min="4" max="4" width="18" customWidth="1"/>
+    <col min="4" max="5" width="18" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>6</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="16">
       <c r="A2" s="2" t="s">
-        <v>48</v>
+        <v>25</v>
       </c>
       <c r="B2" s="2"/>
-      <c r="C2" s="5" t="s">
-        <v>9</v>
+      <c r="C2" s="3" t="s">
+        <v>7</v>
       </c>
       <c r="D2" s="2"/>
       <c r="E2" s="2" t="s">
@@ -690,251 +763,211 @@
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="2" t="s">
-        <v>48</v>
+        <v>25</v>
       </c>
       <c r="B3" s="2"/>
       <c r="C3" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="E3" s="2"/>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="2" t="s">
-        <v>48</v>
+        <v>25</v>
       </c>
       <c r="B4" s="2"/>
       <c r="C4" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="E4" s="2"/>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" s="2" t="s">
-        <v>48</v>
+        <v>25</v>
       </c>
       <c r="B5" s="2"/>
       <c r="C5" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="E5" s="2"/>
+        <v>11</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" s="2" t="s">
-        <v>48</v>
+        <v>25</v>
       </c>
       <c r="B6" s="2"/>
       <c r="C6" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D6" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="E6" s="2"/>
+        <v>11</v>
+      </c>
+      <c r="D6" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" s="2" t="s">
-        <v>48</v>
+        <v>25</v>
       </c>
       <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="3"/>
+      <c r="C7" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>24</v>
+      </c>
       <c r="E7" s="2"/>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" s="2" t="s">
-        <v>8</v>
+        <v>25</v>
       </c>
       <c r="B8" s="2"/>
       <c r="C8" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>20</v>
+        <v>11</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>31</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>23</v>
+        <v>34</v>
       </c>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" s="2" t="s">
-        <v>8</v>
+        <v>25</v>
       </c>
       <c r="B9" s="2"/>
-      <c r="C9" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>24</v>
-      </c>
+      <c r="C9" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="E9" s="2"/>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" s="2" t="s">
-        <v>8</v>
+        <v>25</v>
       </c>
       <c r="B10" s="2"/>
-      <c r="C10" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="E10" s="2"/>
+      <c r="C10" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="D10" s="5"/>
+      <c r="E10" s="13" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" s="2" t="s">
-        <v>8</v>
+        <v>25</v>
       </c>
       <c r="B11" s="2"/>
       <c r="C11" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
+        <v>11</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="12" spans="1:5">
       <c r="A12" s="2" t="s">
-        <v>8</v>
+        <v>25</v>
       </c>
       <c r="B12" s="2"/>
-      <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
-      <c r="E12" s="2"/>
+      <c r="C12" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="13" spans="1:5">
-      <c r="A13" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="C13" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="D13" s="7"/>
-      <c r="E13" t="s">
-        <v>1</v>
+      <c r="A13" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B13" s="2"/>
+      <c r="C13" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="14" spans="1:5">
-      <c r="A14" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="C14" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="D14" t="s">
-        <v>17</v>
-      </c>
+      <c r="A14" s="2"/>
+      <c r="B14" s="2"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
     </row>
     <row r="15" spans="1:5">
-      <c r="A15" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="C15" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="D15" t="s">
-        <v>18</v>
-      </c>
-      <c r="E15" s="7"/>
+      <c r="A15" s="2"/>
+      <c r="C15" s="4"/>
+      <c r="D15" s="5"/>
     </row>
     <row r="16" spans="1:5">
-      <c r="A16" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="C16" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="D16" t="s">
-        <v>19</v>
-      </c>
+      <c r="A16" s="7"/>
+      <c r="C16" s="8"/>
     </row>
     <row r="17" spans="1:5">
-      <c r="A17" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="C17" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="D17" t="s">
-        <v>34</v>
-      </c>
+      <c r="A17" s="7"/>
+      <c r="C17" s="8"/>
+      <c r="E17" s="5"/>
     </row>
     <row r="18" spans="1:5">
-      <c r="A18" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="C18" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="D18" t="s">
-        <v>35</v>
-      </c>
+      <c r="A18" s="7"/>
+      <c r="C18" s="8"/>
     </row>
     <row r="19" spans="1:5">
-      <c r="A19" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="C19" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="D19" t="s">
-        <v>36</v>
-      </c>
+      <c r="A19" s="7"/>
+      <c r="C19" s="8"/>
     </row>
     <row r="20" spans="1:5">
-      <c r="A20" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="C20" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="D20" t="s">
-        <v>37</v>
-      </c>
-      <c r="E20" t="s">
-        <v>39</v>
-      </c>
+      <c r="A20" s="7"/>
+      <c r="C20" s="8"/>
     </row>
     <row r="21" spans="1:5">
-      <c r="A21" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="C21" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="D21" t="s">
-        <v>38</v>
-      </c>
-      <c r="E21" t="s">
-        <v>40</v>
-      </c>
+      <c r="A21" s="7"/>
+      <c r="C21" s="8"/>
     </row>
     <row r="22" spans="1:5">
-      <c r="A22" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="C22" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="D22" t="s">
-        <v>42</v>
-      </c>
-      <c r="E22" t="s">
-        <v>41</v>
-      </c>
+      <c r="A22" s="7"/>
+      <c r="C22" s="8"/>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="A23" s="7"/>
+      <c r="C23" s="8"/>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="A24" s="7"/>
+      <c r="C24" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -945,155 +978,136 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:J11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F30" sqref="F30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
+    <col min="1" max="2" width="13.83203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15.1640625" customWidth="1"/>
+    <col min="9" max="9" width="16.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
-      <c r="A1" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5">
+    <row r="1" spans="1:10">
+      <c r="A1" s="11" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>24</v>
+        <v>38</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>1</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
+        <v>16</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="J2" s="2"/>
+    </row>
+    <row r="3" spans="1:10">
       <c r="A3" t="s">
         <v>2</v>
       </c>
       <c r="B3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F3" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="C3" t="s">
-        <v>45</v>
-      </c>
-      <c r="D3" t="s">
-        <v>30</v>
-      </c>
-      <c r="E3" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="A4" t="s">
-        <v>29</v>
-      </c>
-      <c r="B4" t="s">
-        <v>44</v>
-      </c>
-      <c r="C4" t="s">
+      <c r="G3" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="H3" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="I3" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="D4" t="s">
-        <v>3</v>
-      </c>
-      <c r="E4" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
-      <c r="A5" t="s">
-        <v>29</v>
-      </c>
-      <c r="B5" t="s">
-        <v>26</v>
-      </c>
-      <c r="C5" t="s">
-        <v>26</v>
-      </c>
-      <c r="D5" t="s">
-        <v>28</v>
-      </c>
-      <c r="E5" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5">
-      <c r="A6" t="s">
-        <v>29</v>
-      </c>
-      <c r="B6" t="s">
-        <v>26</v>
-      </c>
-      <c r="C6" t="s">
-        <v>26</v>
-      </c>
-      <c r="D6" t="s">
-        <v>3</v>
-      </c>
-      <c r="E6" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5">
+    </row>
+    <row r="4" spans="1:10">
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+    </row>
+    <row r="8" spans="1:10">
       <c r="A8" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10">
       <c r="A9" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>1</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10">
       <c r="A10" t="s">
         <v>2</v>
       </c>
       <c r="B10" t="s">
-        <v>30</v>
-      </c>
-      <c r="C10" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="D10" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="E10" s="8" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5">
+        <v>20</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10">
       <c r="A11" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="B11" t="s">
-        <v>26</v>
-      </c>
-      <c r="C11" s="8" t="s">
-        <v>26</v>
+        <v>17</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated GenericKey, Keywords, Xles Set data
</commit_message>
<xml_diff>
--- a/data/TestData.xlsx
+++ b/data/TestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27022"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1500" yWindow="0" windowWidth="28560" windowHeight="28320" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="1500" yWindow="0" windowWidth="36000" windowHeight="28320" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="TestCases" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="51">
   <si>
     <t>Runmode</t>
   </si>
@@ -157,20 +157,29 @@
     <t>nextStep_cssSelector</t>
   </si>
   <si>
-    <t>10</t>
-  </si>
-  <si>
     <t>02/01/2017</t>
   </si>
   <si>
     <t>1/1/2015</t>
+  </si>
+  <si>
+    <t>getVisibleElementCount</t>
+  </si>
+  <si>
+    <t>ExpectedData</t>
+  </si>
+  <si>
+    <t>ActualData</t>
+  </si>
+  <si>
+    <t>5</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -197,12 +206,6 @@
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
-      <name val="Menlo"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="9"/>
-      <color rgb="FF008000"/>
       <name val="Menlo"/>
     </font>
     <font>
@@ -244,7 +247,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -278,8 +281,21 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="41">
+  <cellStyleXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -321,8 +337,12 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -332,23 +352,30 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="41">
+  <cellStyles count="45">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -369,6 +396,8 @@
     <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -389,6 +418,8 @@
     <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -718,20 +749,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E24"/>
+  <dimension ref="A1:G24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="13.83203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.6640625" customWidth="1"/>
-    <col min="4" max="5" width="18" customWidth="1"/>
+    <col min="1" max="1" width="13.83203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="20.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="18" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="13.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="9.83203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="15" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
@@ -747,8 +781,14 @@
       <c r="E1" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" ht="16">
+      <c r="F1" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="16">
       <c r="A2" s="2" t="s">
         <v>25</v>
       </c>
@@ -757,11 +797,12 @@
         <v>7</v>
       </c>
       <c r="D2" s="2"/>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="16" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:5">
+      <c r="F2" s="14"/>
+    </row>
+    <row r="3" spans="1:7">
       <c r="A3" s="2" t="s">
         <v>25</v>
       </c>
@@ -773,8 +814,9 @@
         <v>12</v>
       </c>
       <c r="E3" s="2"/>
-    </row>
-    <row r="4" spans="1:5">
+      <c r="F3" s="14"/>
+    </row>
+    <row r="4" spans="1:7">
       <c r="A4" s="2" t="s">
         <v>25</v>
       </c>
@@ -786,8 +828,9 @@
         <v>13</v>
       </c>
       <c r="E4" s="2"/>
-    </row>
-    <row r="5" spans="1:5">
+      <c r="F4" s="14"/>
+    </row>
+    <row r="5" spans="1:7">
       <c r="A5" s="2" t="s">
         <v>25</v>
       </c>
@@ -795,14 +838,15 @@
       <c r="C5" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D5" s="9" t="s">
+      <c r="D5" s="8" t="s">
         <v>26</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="6" spans="1:5">
+      <c r="F5" s="14"/>
+    </row>
+    <row r="6" spans="1:7">
       <c r="A6" s="2" t="s">
         <v>25</v>
       </c>
@@ -810,14 +854,15 @@
       <c r="C6" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D6" s="9" t="s">
+      <c r="D6" s="8" t="s">
         <v>27</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="7" spans="1:5">
+      <c r="F6" s="14"/>
+    </row>
+    <row r="7" spans="1:7">
       <c r="A7" s="2" t="s">
         <v>25</v>
       </c>
@@ -825,12 +870,13 @@
       <c r="C7" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D7" s="9" t="s">
+      <c r="D7" s="8" t="s">
         <v>24</v>
       </c>
       <c r="E7" s="2"/>
-    </row>
-    <row r="8" spans="1:5">
+      <c r="F7" s="14"/>
+    </row>
+    <row r="8" spans="1:7">
       <c r="A8" s="2" t="s">
         <v>25</v>
       </c>
@@ -838,40 +884,43 @@
       <c r="C8" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D8" s="5" t="s">
+      <c r="D8" s="4" t="s">
         <v>31</v>
       </c>
       <c r="E8" s="2" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="9" spans="1:5">
+      <c r="F8" s="14"/>
+    </row>
+    <row r="9" spans="1:7">
       <c r="A9" s="2" t="s">
         <v>25</v>
       </c>
       <c r="B9" s="2"/>
-      <c r="C9" s="7" t="s">
+      <c r="C9" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="D9" s="5" t="s">
+      <c r="D9" s="4" t="s">
         <v>44</v>
       </c>
       <c r="E9" s="2"/>
-    </row>
-    <row r="10" spans="1:5">
+      <c r="F9" s="14"/>
+    </row>
+    <row r="10" spans="1:7">
       <c r="A10" s="2" t="s">
         <v>25</v>
       </c>
       <c r="B10" s="2"/>
-      <c r="C10" s="12" t="s">
+      <c r="C10" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="D10" s="5"/>
-      <c r="E10" s="13" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5">
+      <c r="D10" s="4"/>
+      <c r="E10" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="F10" s="15"/>
+    </row>
+    <row r="11" spans="1:7">
       <c r="A11" s="2" t="s">
         <v>25</v>
       </c>
@@ -879,14 +928,15 @@
       <c r="C11" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D11" s="5" t="s">
+      <c r="D11" s="4" t="s">
         <v>32</v>
       </c>
       <c r="E11" s="2" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="12" spans="1:5">
+      <c r="F11" s="14"/>
+    </row>
+    <row r="12" spans="1:7">
       <c r="A12" s="2" t="s">
         <v>25</v>
       </c>
@@ -894,76 +944,94 @@
       <c r="C12" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D12" s="5" t="s">
+      <c r="D12" s="4" t="s">
         <v>33</v>
       </c>
       <c r="E12" s="2" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="13" spans="1:5">
+      <c r="F12" s="14"/>
+    </row>
+    <row r="13" spans="1:7">
       <c r="A13" s="2" t="s">
         <v>25</v>
       </c>
       <c r="B13" s="2"/>
-      <c r="C13" s="7" t="s">
+      <c r="C13" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="D13" s="5" t="s">
+      <c r="D13" s="4" t="s">
         <v>39</v>
       </c>
       <c r="E13" s="2" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="14" spans="1:5">
-      <c r="A14" s="2"/>
+      <c r="F13" s="14"/>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="A14" s="2" t="s">
+        <v>25</v>
+      </c>
       <c r="B14" s="2"/>
-      <c r="C14" s="2"/>
+      <c r="C14" s="11" t="s">
+        <v>47</v>
+      </c>
       <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
-    </row>
-    <row r="15" spans="1:5">
-      <c r="A15" s="2"/>
-      <c r="C15" s="4"/>
-      <c r="D15" s="5"/>
-    </row>
-    <row r="16" spans="1:5">
-      <c r="A16" s="7"/>
-      <c r="C16" s="8"/>
-    </row>
-    <row r="17" spans="1:5">
-      <c r="A17" s="7"/>
-      <c r="C17" s="8"/>
-      <c r="E17" s="5"/>
-    </row>
-    <row r="18" spans="1:5">
-      <c r="A18" s="7"/>
-      <c r="C18" s="8"/>
-    </row>
-    <row r="19" spans="1:5">
-      <c r="A19" s="7"/>
-      <c r="C19" s="8"/>
-    </row>
-    <row r="20" spans="1:5">
-      <c r="A20" s="7"/>
-      <c r="C20" s="8"/>
-    </row>
-    <row r="21" spans="1:5">
-      <c r="A21" s="7"/>
-      <c r="C21" s="8"/>
-    </row>
-    <row r="22" spans="1:5">
-      <c r="A22" s="7"/>
-      <c r="C22" s="8"/>
-    </row>
-    <row r="23" spans="1:5">
-      <c r="A23" s="7"/>
-      <c r="C23" s="8"/>
-    </row>
-    <row r="24" spans="1:5">
-      <c r="A24" s="7"/>
-      <c r="C24" s="8"/>
+      <c r="E14" s="13"/>
+      <c r="F14" s="18"/>
+      <c r="G14" s="17" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="A15" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B15" s="2"/>
+      <c r="C15" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7">
+      <c r="A16" s="6"/>
+      <c r="C16" s="7"/>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="A17" s="6"/>
+      <c r="C17" s="7"/>
+      <c r="E17" s="4"/>
+      <c r="F17" s="4"/>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="A18" s="6"/>
+      <c r="C18" s="7"/>
+    </row>
+    <row r="19" spans="1:6">
+      <c r="A19" s="6"/>
+      <c r="C19" s="7"/>
+    </row>
+    <row r="20" spans="1:6">
+      <c r="A20" s="6"/>
+      <c r="C20" s="7"/>
+    </row>
+    <row r="21" spans="1:6">
+      <c r="A21" s="6"/>
+      <c r="C21" s="7"/>
+    </row>
+    <row r="22" spans="1:6">
+      <c r="A22" s="6"/>
+      <c r="C22" s="7"/>
+    </row>
+    <row r="23" spans="1:6">
+      <c r="A23" s="6"/>
+      <c r="C23" s="7"/>
+    </row>
+    <row r="24" spans="1:6">
+      <c r="A24" s="6"/>
+      <c r="C24" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -980,19 +1048,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F30" sqref="F30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="2" width="13.83203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.1640625" customWidth="1"/>
-    <col min="9" max="9" width="16.6640625" customWidth="1"/>
+    <col min="1" max="2" width="13.83203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="15.1640625" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="16.6640625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="10" t="s">
         <v>25</v>
       </c>
     </row>
@@ -1042,17 +1110,17 @@
       <c r="E3" t="s">
         <v>18</v>
       </c>
-      <c r="F3" s="10" t="s">
+      <c r="F3" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="G3" s="10" t="s">
+      <c r="G3" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="H3" s="10" t="s">
-        <v>47</v>
-      </c>
-      <c r="I3" s="10" t="s">
+      <c r="H3" s="9" t="s">
         <v>46</v>
+      </c>
+      <c r="I3" s="9" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -1089,13 +1157,13 @@
       <c r="B10" t="s">
         <v>20</v>
       </c>
-      <c r="C10" s="6" t="s">
+      <c r="C10" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="D10" s="6" t="s">
+      <c r="D10" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="E10" s="6" t="s">
+      <c r="E10" s="5" t="s">
         <v>22</v>
       </c>
     </row>
@@ -1106,7 +1174,7 @@
       <c r="B11" t="s">
         <v>17</v>
       </c>
-      <c r="C11" s="6" t="s">
+      <c r="C11" s="5" t="s">
         <v>17</v>
       </c>
     </row>

</xml_diff>

<commit_message>
We've finished Check Eligibility issue
</commit_message>
<xml_diff>
--- a/data/TestData.xlsx
+++ b/data/TestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27022"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="0" windowWidth="28560" windowHeight="28340" tabRatio="500"/>
+    <workbookView xWindow="240" yWindow="0" windowWidth="25060" windowHeight="28340" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="TestCases" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="64">
   <si>
     <t>Runmode</t>
   </si>
@@ -151,9 +151,6 @@
     <t>ActualData</t>
   </si>
   <si>
-    <t>5</t>
-  </si>
-  <si>
     <t>cheatButton_id</t>
   </si>
   <si>
@@ -205,13 +202,16 @@
     <t>State_id</t>
   </si>
   <si>
-    <t/>
-  </si>
-  <si>
     <t>Status</t>
   </si>
   <si>
-    <t>GetStateCode</t>
+    <t>selectDpsd</t>
+  </si>
+  <si>
+    <t>getStateCode</t>
+  </si>
+  <si>
+    <t>08406</t>
   </si>
 </sst>
 </file>
@@ -347,7 +347,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="101">
+  <cellStyleXfs count="111">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -449,8 +449,18 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -476,7 +486,6 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -495,6 +504,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -502,7 +517,7 @@
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="101">
+  <cellStyles count="111">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -553,6 +568,11 @@
     <cellStyle name="Followed Hyperlink" xfId="96" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="98" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="100" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="102" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="104" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="106" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="108" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="110" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -603,6 +623,11 @@
     <cellStyle name="Hyperlink" xfId="95" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="97" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="99" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="101" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="103" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="105" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="107" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="109" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -932,10 +957,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H31"/>
+  <dimension ref="A1:H30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="G31" sqref="G31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -959,7 +984,7 @@
       <c r="C1" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="18" t="s">
+      <c r="D1" s="17" t="s">
         <v>17</v>
       </c>
       <c r="E1" s="1" t="s">
@@ -971,8 +996,8 @@
       <c r="G1" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="H1" s="23" t="s">
-        <v>62</v>
+      <c r="H1" s="22" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="16">
@@ -983,7 +1008,7 @@
       <c r="C2" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="19"/>
+      <c r="D2" s="18"/>
       <c r="E2" s="2" t="s">
         <v>1</v>
       </c>
@@ -998,7 +1023,7 @@
       <c r="C3" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="19" t="s">
+      <c r="D3" s="18" t="s">
         <v>12</v>
       </c>
       <c r="E3" s="2"/>
@@ -1013,7 +1038,7 @@
       <c r="C4" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="19" t="s">
+      <c r="D4" s="18" t="s">
         <v>13</v>
       </c>
       <c r="E4" s="2"/>
@@ -1026,9 +1051,9 @@
       </c>
       <c r="B5" s="2"/>
       <c r="C5" s="15" t="s">
-        <v>52</v>
-      </c>
-      <c r="D5" s="20" t="s">
+        <v>51</v>
+      </c>
+      <c r="D5" s="19" t="s">
         <v>19</v>
       </c>
       <c r="E5" s="2" t="s">
@@ -1043,9 +1068,9 @@
       </c>
       <c r="B6" s="2"/>
       <c r="C6" s="15" t="s">
-        <v>52</v>
-      </c>
-      <c r="D6" s="20" t="s">
+        <v>51</v>
+      </c>
+      <c r="D6" s="19" t="s">
         <v>20</v>
       </c>
       <c r="E6" s="2" t="s">
@@ -1063,7 +1088,7 @@
         <v>10</v>
       </c>
       <c r="D7" s="10" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
@@ -1074,16 +1099,18 @@
         <v>18</v>
       </c>
       <c r="B8" s="2"/>
-      <c r="C8" s="22" t="s">
+      <c r="C8" s="21" t="s">
         <v>40</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>33</v>
       </c>
       <c r="E8" s="9"/>
-      <c r="F8" s="26"/>
+      <c r="F8" s="26" t="s">
+        <v>56</v>
+      </c>
       <c r="G8" s="6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="9" spans="1:8">
@@ -1091,16 +1118,18 @@
         <v>18</v>
       </c>
       <c r="B9" s="2"/>
-      <c r="C9" s="22" t="s">
+      <c r="C9" s="21" t="s">
         <v>40</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E9" s="9"/>
-      <c r="F9" s="27"/>
+      <c r="F9" s="27" t="s">
+        <v>58</v>
+      </c>
       <c r="G9" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="10" spans="1:8">
@@ -1111,30 +1140,30 @@
       <c r="C10" s="15" t="s">
         <v>52</v>
       </c>
-      <c r="D10" s="20" t="s">
-        <v>24</v>
+      <c r="D10" s="19" t="s">
+        <v>25</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="F10" s="2"/>
-      <c r="G10" s="2"/>
+        <v>28</v>
+      </c>
+      <c r="F10" s="24"/>
+      <c r="G10" s="6"/>
     </row>
     <row r="11" spans="1:8">
       <c r="A11" s="2" t="s">
         <v>18</v>
       </c>
       <c r="B11" s="2"/>
-      <c r="C11" s="24" t="s">
-        <v>63</v>
+      <c r="C11" s="2" t="s">
+        <v>53</v>
       </c>
       <c r="D11" s="20" t="s">
-        <v>60</v>
-      </c>
-      <c r="E11" s="6"/>
-      <c r="F11" s="25" t="s">
-        <v>61</v>
-      </c>
+        <v>26</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F11" s="2"/>
       <c r="G11" s="2"/>
     </row>
     <row r="12" spans="1:8">
@@ -1142,13 +1171,15 @@
         <v>18</v>
       </c>
       <c r="B12" s="2"/>
-      <c r="C12" s="17" t="s">
-        <v>10</v>
-      </c>
-      <c r="D12" s="20" t="s">
-        <v>37</v>
-      </c>
-      <c r="E12" s="2"/>
+      <c r="C12" s="15" t="s">
+        <v>51</v>
+      </c>
+      <c r="D12" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>27</v>
+      </c>
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
     </row>
@@ -1157,48 +1188,46 @@
         <v>18</v>
       </c>
       <c r="B13" s="2"/>
-      <c r="C13" s="16" t="s">
-        <v>35</v>
-      </c>
-      <c r="D13" s="20"/>
-      <c r="E13" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="F13" s="6"/>
+      <c r="C13" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D13" s="20" t="s">
+        <v>37</v>
+      </c>
+      <c r="E13" s="2"/>
+      <c r="F13" s="20"/>
       <c r="G13" s="2"/>
+      <c r="H13" s="7"/>
     </row>
     <row r="14" spans="1:8">
       <c r="A14" s="2" t="s">
         <v>18</v>
       </c>
       <c r="B14" s="2"/>
-      <c r="C14" s="15" t="s">
-        <v>53</v>
-      </c>
-      <c r="D14" s="20" t="s">
-        <v>25</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="F14" s="2"/>
+      <c r="C14" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="D14" s="19"/>
+      <c r="E14" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="F14" s="25"/>
       <c r="G14" s="2"/>
+      <c r="H14" s="7"/>
     </row>
     <row r="15" spans="1:8">
       <c r="A15" s="2" t="s">
         <v>18</v>
       </c>
       <c r="B15" s="2"/>
-      <c r="C15" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="D15" s="21" t="s">
-        <v>26</v>
-      </c>
-      <c r="E15" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="F15" s="2"/>
+      <c r="C15" s="23" t="s">
+        <v>62</v>
+      </c>
+      <c r="D15" s="19" t="s">
+        <v>59</v>
+      </c>
+      <c r="E15" s="6"/>
+      <c r="F15" s="28"/>
       <c r="G15" s="2"/>
     </row>
     <row r="16" spans="1:8">
@@ -1206,29 +1235,29 @@
         <v>18</v>
       </c>
       <c r="B16" s="2"/>
-      <c r="C16" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="D16" s="21" t="s">
+      <c r="C16" s="23" t="s">
+        <v>61</v>
+      </c>
+      <c r="D16" s="20" t="s">
         <v>32</v>
       </c>
       <c r="E16" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="F16" s="2"/>
-      <c r="G16" s="2"/>
+      <c r="F16" s="9"/>
+      <c r="G16" s="6"/>
     </row>
     <row r="17" spans="1:8">
       <c r="A17" s="2" t="s">
         <v>18</v>
       </c>
       <c r="B17" s="2"/>
-      <c r="C17" s="22" t="s">
+      <c r="C17" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="D17" s="21"/>
+      <c r="D17" s="20"/>
       <c r="E17" s="6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F17" s="2"/>
       <c r="G17" s="2"/>
@@ -1238,37 +1267,33 @@
         <v>18</v>
       </c>
       <c r="B18" s="2"/>
-      <c r="C18" s="22" t="s">
-        <v>40</v>
-      </c>
-      <c r="D18" s="2"/>
-      <c r="E18" s="9"/>
-      <c r="F18" s="9"/>
-      <c r="G18" s="6" t="s">
-        <v>43</v>
-      </c>
+      <c r="C18" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D18" s="20" t="s">
+        <v>37</v>
+      </c>
+      <c r="E18" s="2"/>
+      <c r="F18" s="20"/>
+      <c r="G18" s="2"/>
+      <c r="H18" s="7"/>
     </row>
     <row r="19" spans="1:8">
-      <c r="A19" s="2" t="s">
-        <v>18</v>
-      </c>
+      <c r="A19" s="2"/>
       <c r="B19" s="2"/>
-      <c r="C19" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="D19" s="21" t="s">
-        <v>37</v>
-      </c>
-      <c r="E19" s="2"/>
+      <c r="C19" s="21"/>
+      <c r="D19" s="20"/>
+      <c r="E19" s="8"/>
       <c r="F19" s="2"/>
       <c r="G19" s="2"/>
+      <c r="H19" s="7"/>
     </row>
     <row r="20" spans="1:8">
       <c r="A20" s="2"/>
       <c r="B20" s="2"/>
-      <c r="C20" s="22"/>
-      <c r="D20" s="21"/>
-      <c r="E20" s="8"/>
+      <c r="C20" s="2"/>
+      <c r="D20" s="2"/>
+      <c r="E20" s="20"/>
       <c r="F20" s="2"/>
       <c r="G20" s="2"/>
       <c r="H20" s="7"/>
@@ -1278,19 +1303,19 @@
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
-      <c r="E21" s="21"/>
-      <c r="F21" s="21"/>
+      <c r="E21" s="2"/>
+      <c r="F21" s="2"/>
       <c r="G21" s="2"/>
       <c r="H21" s="7"/>
     </row>
     <row r="22" spans="1:8">
-      <c r="A22" s="2"/>
-      <c r="B22" s="2"/>
-      <c r="C22" s="2"/>
-      <c r="D22" s="2"/>
-      <c r="E22" s="2"/>
-      <c r="F22" s="2"/>
-      <c r="G22" s="2"/>
+      <c r="A22" s="3"/>
+      <c r="B22" s="3"/>
+      <c r="C22" s="7"/>
+      <c r="D22" s="7"/>
+      <c r="E22" s="7"/>
+      <c r="F22" s="7"/>
+      <c r="G22" s="7"/>
       <c r="H22" s="7"/>
     </row>
     <row r="23" spans="1:8">
@@ -1344,8 +1369,8 @@
       <c r="H27" s="7"/>
     </row>
     <row r="28" spans="1:8">
-      <c r="A28" s="3"/>
-      <c r="B28" s="3"/>
+      <c r="A28" s="7"/>
+      <c r="B28" s="7"/>
       <c r="C28" s="7"/>
       <c r="D28" s="7"/>
       <c r="E28" s="7"/>
@@ -1359,9 +1384,6 @@
       <c r="C29" s="7"/>
       <c r="D29" s="7"/>
       <c r="E29" s="7"/>
-      <c r="F29" s="7"/>
-      <c r="G29" s="7"/>
-      <c r="H29" s="7"/>
     </row>
     <row r="30" spans="1:8">
       <c r="A30" s="7"/>
@@ -1369,19 +1391,6 @@
       <c r="C30" s="7"/>
       <c r="D30" s="7"/>
       <c r="E30" s="7"/>
-      <c r="F30" s="7"/>
-      <c r="G30" s="7"/>
-      <c r="H30" s="7"/>
-    </row>
-    <row r="31" spans="1:8">
-      <c r="A31" s="7"/>
-      <c r="B31" s="7"/>
-      <c r="C31" s="7"/>
-      <c r="D31" s="7"/>
-      <c r="E31" s="7"/>
-      <c r="F31" s="7"/>
-      <c r="G31" s="7"/>
-      <c r="H31" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1399,7 +1408,7 @@
   <dimension ref="A1:J12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+      <selection activeCell="E33" sqref="E33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1464,21 +1473,21 @@
         <v>36</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="I3" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="4" spans="1:10">
-      <c r="A4" s="7" t="s">
+      <c r="A4" t="s">
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C4" t="s">
         <v>23</v>
@@ -1490,21 +1499,21 @@
         <v>15</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>36</v>
+        <v>63</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="I4" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="7" spans="1:10">
       <c r="A7" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="8" spans="1:10">
@@ -1568,10 +1577,10 @@
     </row>
     <row r="10" spans="1:10">
       <c r="A10" s="7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C10" t="s">
         <v>23</v>
@@ -1583,7 +1592,7 @@
         <v>15</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G10" s="4" t="s">
         <v>30</v>

</xml_diff>

<commit_message>
Initial commit of this framework
</commit_message>
<xml_diff>
--- a/data/TestData.xlsx
+++ b/data/TestData.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27022"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="0" windowWidth="20730" windowHeight="11760" tabRatio="500"/>
+    <workbookView xWindow="240" yWindow="0" windowWidth="20900" windowHeight="28340" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="TestCases" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="79">
   <si>
     <t>Runmode</t>
   </si>
@@ -263,6 +263,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="0"/>
   <fonts count="8">
     <font>
       <sz val="12"/>
@@ -312,10 +313,8 @@
     </font>
     <font>
       <b/>
-      <sz val="9"/>
-      <color rgb="FF000080"/>
-      <name val="Courier New"/>
-      <family val="3"/>
+      <sz val="10"/>
+      <name val="Arial"/>
     </font>
   </fonts>
   <fills count="4">
@@ -512,7 +511,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -525,9 +524,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
@@ -538,11 +534,6 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -559,12 +550,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -577,6 +562,38 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment wrapText="true"/>
     </xf>
   </cellXfs>
   <cellStyles count="111">
@@ -1026,19 +1043,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="E26" sqref="E26:I27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="19.875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="19.875" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="18.625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="19" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="13.5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="9.875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="32.625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="19.83203125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="19.83203125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="18.6640625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="33" width="50.83203125" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="13.5" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="9.8671875" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="32.6640625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -1048,10 +1065,10 @@
       <c r="B1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="13" t="s">
+      <c r="C1" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="17" t="s">
+      <c r="D1" s="27" t="s">
         <v>17</v>
       </c>
       <c r="E1" s="1" t="s">
@@ -1063,19 +1080,19 @@
       <c r="G1" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="H1" s="22" t="s">
+      <c r="H1" s="18" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" ht="16">
       <c r="A2" s="2" t="s">
         <v>18</v>
       </c>
       <c r="B2" s="2"/>
-      <c r="C2" s="14" t="s">
+      <c r="C2" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="18"/>
+      <c r="D2" s="28"/>
       <c r="E2" s="2" t="s">
         <v>1</v>
       </c>
@@ -1087,10 +1104,10 @@
         <v>18</v>
       </c>
       <c r="B3" s="2"/>
-      <c r="C3" s="15" t="s">
+      <c r="C3" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="18" t="s">
+      <c r="D3" s="28" t="s">
         <v>12</v>
       </c>
       <c r="E3" s="2"/>
@@ -1102,10 +1119,10 @@
         <v>18</v>
       </c>
       <c r="B4" s="2"/>
-      <c r="C4" s="15" t="s">
+      <c r="C4" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="18" t="s">
+      <c r="D4" s="28" t="s">
         <v>13</v>
       </c>
       <c r="E4" s="2"/>
@@ -1117,10 +1134,10 @@
         <v>18</v>
       </c>
       <c r="B5" s="2"/>
-      <c r="C5" s="15" t="s">
+      <c r="C5" s="14" t="s">
         <v>51</v>
       </c>
-      <c r="D5" s="19" t="s">
+      <c r="D5" s="29" t="s">
         <v>19</v>
       </c>
       <c r="E5" s="2" t="s">
@@ -1134,10 +1151,10 @@
         <v>18</v>
       </c>
       <c r="B6" s="2"/>
-      <c r="C6" s="15" t="s">
+      <c r="C6" s="14" t="s">
         <v>51</v>
       </c>
-      <c r="D6" s="19" t="s">
+      <c r="D6" s="29" t="s">
         <v>20</v>
       </c>
       <c r="E6" s="2" t="s">
@@ -1151,10 +1168,10 @@
         <v>18</v>
       </c>
       <c r="B7" s="2"/>
-      <c r="C7" s="15" t="s">
+      <c r="C7" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="D7" s="10" t="s">
+      <c r="D7" s="30" t="s">
         <v>43</v>
       </c>
       <c r="E7" s="2"/>
@@ -1166,14 +1183,14 @@
         <v>18</v>
       </c>
       <c r="B8" s="2"/>
-      <c r="C8" s="21" t="s">
+      <c r="C8" s="17" t="s">
         <v>40</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="D8" s="31" t="s">
         <v>33</v>
       </c>
       <c r="E8" s="9"/>
-      <c r="F8" s="30" t="s">
+      <c r="F8" s="38" t="s">
         <v>56</v>
       </c>
       <c r="G8" s="6" t="s">
@@ -1185,14 +1202,14 @@
         <v>18</v>
       </c>
       <c r="B9" s="2"/>
-      <c r="C9" s="21" t="s">
+      <c r="C9" s="17" t="s">
         <v>40</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="D9" s="31" t="s">
         <v>11</v>
       </c>
       <c r="E9" s="9"/>
-      <c r="F9" s="31" t="s">
+      <c r="F9" s="39" t="s">
         <v>58</v>
       </c>
       <c r="G9" s="6" t="s">
@@ -1204,16 +1221,16 @@
         <v>18</v>
       </c>
       <c r="B10" s="2"/>
-      <c r="C10" s="15" t="s">
+      <c r="C10" s="14" t="s">
         <v>52</v>
       </c>
-      <c r="D10" s="19" t="s">
+      <c r="D10" s="29" t="s">
         <v>25</v>
       </c>
       <c r="E10" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="F10" s="24"/>
+      <c r="F10" s="20"/>
       <c r="G10" s="6"/>
     </row>
     <row r="11" spans="1:8">
@@ -1224,7 +1241,7 @@
       <c r="C11" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="D11" s="20" t="s">
+      <c r="D11" s="32" t="s">
         <v>26</v>
       </c>
       <c r="E11" s="2" t="s">
@@ -1238,10 +1255,10 @@
         <v>18</v>
       </c>
       <c r="B12" s="2"/>
-      <c r="C12" s="15" t="s">
+      <c r="C12" s="14" t="s">
         <v>51</v>
       </c>
-      <c r="D12" s="19" t="s">
+      <c r="D12" s="29" t="s">
         <v>24</v>
       </c>
       <c r="E12" s="2" t="s">
@@ -1258,11 +1275,11 @@
       <c r="C13" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="D13" s="20" t="s">
+      <c r="D13" s="32" t="s">
         <v>37</v>
       </c>
       <c r="E13" s="2"/>
-      <c r="F13" s="20"/>
+      <c r="F13" s="16"/>
       <c r="G13" s="2"/>
       <c r="H13" s="7"/>
     </row>
@@ -1271,14 +1288,14 @@
         <v>18</v>
       </c>
       <c r="B14" s="2"/>
-      <c r="C14" s="16" t="s">
+      <c r="C14" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="D14" s="19"/>
+      <c r="D14" s="29"/>
       <c r="E14" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="F14" s="25"/>
+      <c r="F14" s="21"/>
       <c r="G14" s="2"/>
       <c r="H14" s="7"/>
     </row>
@@ -1287,14 +1304,14 @@
         <v>18</v>
       </c>
       <c r="B15" s="2"/>
-      <c r="C15" s="23" t="s">
+      <c r="C15" s="19" t="s">
         <v>62</v>
       </c>
-      <c r="D15" s="19" t="s">
+      <c r="D15" s="29" t="s">
         <v>59</v>
       </c>
       <c r="E15" s="6"/>
-      <c r="F15" s="32" t="s">
+      <c r="F15" s="40" t="s">
         <v>78</v>
       </c>
       <c r="G15" s="2"/>
@@ -1304,10 +1321,10 @@
         <v>18</v>
       </c>
       <c r="B16" s="2"/>
-      <c r="C16" s="23" t="s">
+      <c r="C16" s="19" t="s">
         <v>61</v>
       </c>
-      <c r="D16" s="20" t="s">
+      <c r="D16" s="32" t="s">
         <v>32</v>
       </c>
       <c r="E16" s="2" t="s">
@@ -1321,10 +1338,10 @@
         <v>18</v>
       </c>
       <c r="B17" s="2"/>
-      <c r="C17" s="21" t="s">
+      <c r="C17" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="D17" s="20"/>
+      <c r="D17" s="32"/>
       <c r="E17" s="6" t="s">
         <v>44</v>
       </c>
@@ -1339,11 +1356,11 @@
       <c r="C18" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="D18" s="20" t="s">
+      <c r="D18" s="32" t="s">
         <v>37</v>
       </c>
       <c r="E18" s="2"/>
-      <c r="F18" s="20"/>
+      <c r="F18" s="16"/>
       <c r="G18" s="2"/>
       <c r="H18" s="7"/>
     </row>
@@ -1354,10 +1371,10 @@
       <c r="B19" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="C19" s="21" t="s">
+      <c r="C19" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="D19" s="20" t="s">
+      <c r="D19" s="32" t="s">
         <v>65</v>
       </c>
       <c r="E19" s="8"/>
@@ -1372,10 +1389,10 @@
       <c r="B20" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="C20" s="21" t="s">
+      <c r="C20" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="D20" s="27" t="s">
+      <c r="D20" s="30" t="s">
         <v>71</v>
       </c>
       <c r="E20" s="8"/>
@@ -1390,11 +1407,11 @@
       <c r="B21" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="C21" s="21" t="s">
+      <c r="C21" s="17" t="s">
         <v>68</v>
       </c>
-      <c r="D21" s="27"/>
-      <c r="E21" s="28" t="s">
+      <c r="D21" s="30"/>
+      <c r="E21" s="22" t="s">
         <v>56</v>
       </c>
       <c r="F21" s="2"/>
@@ -1408,13 +1425,13 @@
       <c r="B22" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="C22" s="21" t="s">
+      <c r="C22" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="D22" s="27" t="s">
+      <c r="D22" s="30" t="s">
         <v>72</v>
       </c>
-      <c r="E22" s="28"/>
+      <c r="E22" s="22"/>
       <c r="F22" s="2"/>
       <c r="G22" s="2"/>
       <c r="H22" s="7"/>
@@ -1426,11 +1443,11 @@
       <c r="B23" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="C23" s="21" t="s">
+      <c r="C23" s="17" t="s">
         <v>68</v>
       </c>
-      <c r="D23" s="27"/>
-      <c r="E23" s="28" t="s">
+      <c r="D23" s="30"/>
+      <c r="E23" s="22" t="s">
         <v>56</v>
       </c>
       <c r="F23" s="2"/>
@@ -1444,13 +1461,13 @@
       <c r="B24" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="C24" s="21" t="s">
+      <c r="C24" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="D24" s="27" t="s">
+      <c r="D24" s="30" t="s">
         <v>73</v>
       </c>
-      <c r="E24" s="28"/>
+      <c r="E24" s="22"/>
       <c r="F24" s="2"/>
       <c r="G24" s="2"/>
       <c r="H24" s="7"/>
@@ -1462,11 +1479,11 @@
       <c r="B25" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="C25" s="21" t="s">
+      <c r="C25" s="17" t="s">
         <v>68</v>
       </c>
-      <c r="D25" s="27"/>
-      <c r="E25" s="28" t="s">
+      <c r="D25" s="30"/>
+      <c r="E25" s="22" t="s">
         <v>56</v>
       </c>
       <c r="F25" s="2"/>
@@ -1480,13 +1497,13 @@
       <c r="B26" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="C26" s="21" t="s">
+      <c r="C26" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="D26" t="s">
+      <c r="D26" s="33" t="s">
         <v>74</v>
       </c>
-      <c r="E26" s="29"/>
+      <c r="E26" s="23"/>
       <c r="F26" s="2"/>
       <c r="G26" s="2"/>
       <c r="H26" s="7"/>
@@ -1498,10 +1515,10 @@
       <c r="B27" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="C27" s="21" t="s">
+      <c r="C27" s="17" t="s">
         <v>69</v>
       </c>
-      <c r="D27" s="27" t="s">
+      <c r="D27" s="30" t="s">
         <v>70</v>
       </c>
       <c r="E27" s="8"/>
@@ -1516,10 +1533,10 @@
       <c r="B28" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="C28" s="21" t="s">
+      <c r="C28" s="17" t="s">
         <v>76</v>
       </c>
-      <c r="D28" s="27" t="s">
+      <c r="D28" s="30" t="s">
         <v>77</v>
       </c>
       <c r="E28" s="8"/>
@@ -1534,13 +1551,13 @@
       <c r="B29" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="C29" s="21" t="s">
+      <c r="C29" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="D29" s="26" t="s">
+      <c r="D29" s="34" t="s">
         <v>75</v>
       </c>
-      <c r="E29" s="20"/>
+      <c r="E29" s="16"/>
       <c r="F29" s="2"/>
       <c r="G29" s="2"/>
       <c r="H29" s="7"/>
@@ -1555,7 +1572,7 @@
       <c r="C30" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="D30" s="20" t="s">
+      <c r="D30" s="32" t="s">
         <v>37</v>
       </c>
       <c r="E30" s="2"/>
@@ -1567,7 +1584,7 @@
       <c r="A31" s="3"/>
       <c r="B31" s="3"/>
       <c r="C31" s="7"/>
-      <c r="D31" s="7"/>
+      <c r="D31" s="35"/>
       <c r="E31" s="7"/>
       <c r="F31" s="7"/>
       <c r="G31" s="7"/>
@@ -1577,7 +1594,7 @@
       <c r="A32" s="3"/>
       <c r="B32" s="3"/>
       <c r="C32" s="7"/>
-      <c r="D32" s="7"/>
+      <c r="D32" s="35"/>
       <c r="E32" s="7"/>
       <c r="F32" s="7"/>
       <c r="G32" s="7"/>
@@ -1587,7 +1604,7 @@
       <c r="A33" s="3"/>
       <c r="B33" s="3"/>
       <c r="C33" s="7"/>
-      <c r="D33" s="7"/>
+      <c r="D33" s="35"/>
       <c r="E33" s="7"/>
       <c r="F33" s="7"/>
       <c r="G33" s="7"/>
@@ -1597,7 +1614,7 @@
       <c r="A34" s="3"/>
       <c r="B34" s="3"/>
       <c r="C34" s="7"/>
-      <c r="D34" s="7"/>
+      <c r="D34" s="35"/>
       <c r="E34" s="7"/>
       <c r="F34" s="7"/>
       <c r="G34" s="7"/>
@@ -1607,7 +1624,7 @@
       <c r="A35" s="3"/>
       <c r="B35" s="3"/>
       <c r="C35" s="7"/>
-      <c r="D35" s="7"/>
+      <c r="D35" s="35"/>
       <c r="E35" s="7"/>
       <c r="F35" s="7"/>
       <c r="G35" s="7"/>
@@ -1617,7 +1634,7 @@
       <c r="A36" s="3"/>
       <c r="B36" s="3"/>
       <c r="C36" s="7"/>
-      <c r="D36" s="7"/>
+      <c r="D36" s="35"/>
       <c r="E36" s="7"/>
       <c r="F36" s="7"/>
       <c r="G36" s="7"/>
@@ -1627,7 +1644,7 @@
       <c r="A37" s="7"/>
       <c r="B37" s="7"/>
       <c r="C37" s="7"/>
-      <c r="D37" s="7"/>
+      <c r="D37" s="35"/>
       <c r="E37" s="7"/>
       <c r="F37" s="7"/>
       <c r="G37" s="7"/>
@@ -1637,19 +1654,19 @@
       <c r="A38" s="7"/>
       <c r="B38" s="7"/>
       <c r="C38" s="7"/>
-      <c r="D38" s="7"/>
+      <c r="D38" s="35"/>
       <c r="E38" s="7"/>
     </row>
     <row r="39" spans="1:8">
       <c r="A39" s="7"/>
       <c r="B39" s="7"/>
       <c r="C39" s="7"/>
-      <c r="D39" s="7"/>
+      <c r="D39" s="35"/>
       <c r="E39" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -1666,11 +1683,11 @@
       <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="2" width="13.875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="15.125" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="16.625" customWidth="1" collapsed="1"/>
+    <col min="1" max="2" bestFit="true" customWidth="true" width="13.83203125" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="15.1640625" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="16.6640625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
@@ -1860,18 +1877,18 @@
       </c>
     </row>
     <row r="11" spans="1:10">
-      <c r="A11" s="11"/>
-      <c r="B11" s="11"/>
-      <c r="C11" s="12"/>
-      <c r="D11" s="11"/>
-      <c r="E11" s="11"/>
+      <c r="A11" s="10"/>
+      <c r="B11" s="10"/>
+      <c r="C11" s="11"/>
+      <c r="D11" s="10"/>
+      <c r="E11" s="10"/>
     </row>
     <row r="12" spans="1:10">
-      <c r="A12" s="11"/>
-      <c r="B12" s="11"/>
-      <c r="C12" s="11"/>
-      <c r="D12" s="11"/>
-      <c r="E12" s="11"/>
+      <c r="A12" s="10"/>
+      <c r="B12" s="10"/>
+      <c r="C12" s="10"/>
+      <c r="D12" s="10"/>
+      <c r="E12" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>